<commit_message>
Modificación del cronograma, y se adjunta capuras de Gantt
</commit_message>
<xml_diff>
--- a/Cronograma de actividades polo 360.xlsx
+++ b/Cronograma de actividades polo 360.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROGRAMADOR WEB INA 2017\PLANIFICACION WEB\1-Planificacion de desarrollo Web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aba0651c8285b0df/Escritorio/plantillas grupo 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_BFB817889A202ED8AF873BC0FFFB4D6E7EB0EBF3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFAA004E-DF0B-4D9F-A502-B70139F81FE9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="735" windowWidth="11655" windowHeight="3420"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Nombre de las tareas</t>
   </si>
@@ -114,16 +115,31 @@
     <t>Recursos</t>
   </si>
   <si>
-    <t>Enc Proyecto</t>
-  </si>
-  <si>
-    <t>Analista</t>
+    <t>Paolo</t>
+  </si>
+  <si>
+    <t>Tatiana</t>
+  </si>
+  <si>
+    <t>Diego</t>
+  </si>
+  <si>
+    <t>Yuliana</t>
+  </si>
+  <si>
+    <t>Diego/Tatiana</t>
+  </si>
+  <si>
+    <t>Yanela</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paolo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -523,11 +539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -537,6 +553,7 @@
     <col min="3" max="3" width="13.7109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" style="5" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
     <col min="7" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
@@ -603,7 +620,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -620,7 +637,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -647,7 +664,9 @@
       <c r="D7" s="4">
         <v>4</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -662,7 +681,9 @@
       <c r="D8" s="4">
         <v>4</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
@@ -672,12 +693,14 @@
         <v>3</v>
       </c>
       <c r="C9" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D9" s="4">
         <v>4</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -692,7 +715,9 @@
       <c r="D10" s="4">
         <v>5</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
@@ -718,7 +743,9 @@
       <c r="D12" s="4">
         <v>9</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
@@ -733,7 +760,9 @@
       <c r="D13" s="4">
         <v>11</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -748,7 +777,9 @@
       <c r="D14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
@@ -769,12 +800,14 @@
         <v>11</v>
       </c>
       <c r="C16" s="4">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D16" s="4">
         <v>13</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
@@ -795,12 +828,14 @@
         <v>16</v>
       </c>
       <c r="C18" s="4">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D18" s="4">
         <v>15</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
@@ -821,12 +856,14 @@
         <v>21</v>
       </c>
       <c r="C20" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D20" s="4">
         <v>17</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
@@ -836,12 +873,14 @@
         <v>22</v>
       </c>
       <c r="C21" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D21" s="4">
         <v>17</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
@@ -851,12 +890,14 @@
         <v>19</v>
       </c>
       <c r="C22" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D22" s="4">
         <v>17</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
@@ -866,12 +907,14 @@
         <v>20</v>
       </c>
       <c r="C23" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D23" s="4">
         <v>17</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
@@ -886,7 +929,9 @@
       <c r="D24" s="4">
         <v>18</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25"/>

</xml_diff>